<commit_message>
hopefully not too mess up
</commit_message>
<xml_diff>
--- a/outputs/macthedPVT.xlsx
+++ b/outputs/macthedPVT.xlsx
@@ -480,25 +480,25 @@
         <v>14.7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0004266041277482926</v>
+        <v>0.0003421115390359828</v>
       </c>
       <c r="C2" t="n">
-        <v>1.042384765759605</v>
+        <v>1.04577084683582</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2064893271247987</v>
+        <v>0.2076774839560538</v>
       </c>
       <c r="E2" t="n">
-        <v>1.020729677522177</v>
+        <v>1.021717547934504</v>
       </c>
       <c r="F2" t="n">
-        <v>5.370885516379929</v>
+        <v>5.292284771237033</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01179371433917792</v>
+        <v>0.01204755792671044</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4555112120249172</v>
+        <v>0.4444235584258014</v>
       </c>
     </row>
     <row r="3">
@@ -506,25 +506,25 @@
         <v>64.951256281407</v>
       </c>
       <c r="B3" t="n">
-        <v>1.046857526852807</v>
+        <v>0.9504625596688521</v>
       </c>
       <c r="C3" t="n">
-        <v>1.042878839847572</v>
+        <v>1.046219838812973</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04642440183551673</v>
+        <v>0.0467230893946119</v>
       </c>
       <c r="E3" t="n">
-        <v>1.020695780167727</v>
+        <v>1.0216832787251</v>
       </c>
       <c r="F3" t="n">
-        <v>5.321133547030278</v>
+        <v>5.247898559053662</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01183371886309955</v>
+        <v>0.01208435411134472</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4564392347733146</v>
+        <v>0.4453289920600459</v>
       </c>
     </row>
     <row r="4">
@@ -532,25 +532,25 @@
         <v>115.202512562814</v>
       </c>
       <c r="B4" t="n">
-        <v>5.757485165149273</v>
+        <v>5.370974007370698</v>
       </c>
       <c r="C4" t="n">
-        <v>1.04510297046489</v>
+        <v>1.048308809931147</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02600056710253437</v>
+        <v>0.02618594678366804</v>
       </c>
       <c r="E4" t="n">
-        <v>1.020660592505839</v>
+        <v>1.021647714964968</v>
       </c>
       <c r="F4" t="n">
-        <v>5.108484614230274</v>
+        <v>5.051138252356188</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01188510001150347</v>
+        <v>0.01213170481622541</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4573744033959086</v>
+        <v>0.4462413976298976</v>
       </c>
     </row>
     <row r="5">
@@ -558,25 +558,25 @@
         <v>165.453768844221</v>
       </c>
       <c r="B5" t="n">
-        <v>13.87749282878754</v>
+        <v>13.1282533264224</v>
       </c>
       <c r="C5" t="n">
-        <v>1.048936845490532</v>
+        <v>1.051974614814772</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01798342670081142</v>
+        <v>0.01812445259810562</v>
       </c>
       <c r="E5" t="n">
-        <v>1.020624114536513</v>
+        <v>1.02161085665411</v>
       </c>
       <c r="F5" t="n">
-        <v>4.7804760074475</v>
+        <v>4.740474866237616</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01194422909195253</v>
+        <v>0.01218619533427647</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4583167178926992</v>
+        <v>0.4471607751353562</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
         <v>215.705025125628</v>
       </c>
       <c r="B6" t="n">
-        <v>24.52273512050365</v>
+        <v>23.40974476070298</v>
       </c>
       <c r="C6" t="n">
-        <v>1.053963014215331</v>
+        <v>1.056833269500336</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01370213518520468</v>
+        <v>0.01381956537867458</v>
       </c>
       <c r="E6" t="n">
-        <v>1.02058634625975</v>
+        <v>1.021572703792524</v>
       </c>
       <c r="F6" t="n">
-        <v>4.411338649188032</v>
+        <v>4.385138500960083</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01200977753235727</v>
+        <v>0.0122465572598686</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4592661782636866</v>
+        <v>0.448087124576422</v>
       </c>
     </row>
     <row r="7">
@@ -610,25 +610,25 @@
         <v>265.956281407035</v>
       </c>
       <c r="B7" t="n">
-        <v>37.00060235302222</v>
+        <v>35.5530819094895</v>
       </c>
       <c r="C7" t="n">
-        <v>1.059854459831847</v>
+        <v>1.062571763989531</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01103912053848628</v>
+        <v>0.01114194205861643</v>
       </c>
       <c r="E7" t="n">
-        <v>1.020547287675551</v>
+        <v>1.021533256380211</v>
       </c>
       <c r="F7" t="n">
-        <v>4.047703358833011</v>
+        <v>4.030953007576917</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01208106049108436</v>
+        <v>0.01231212443072353</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4602227845088704</v>
+        <v>0.4490204459530946</v>
       </c>
     </row>
     <row r="8">
@@ -636,25 +636,25 @@
         <v>316.207537688442</v>
       </c>
       <c r="B8" t="n">
-        <v>50.81936319499468</v>
+        <v>49.0782721491173</v>
       </c>
       <c r="C8" t="n">
-        <v>1.066379010580067</v>
+        <v>1.068963271423151</v>
       </c>
       <c r="D8" t="n">
-        <v>0.009222899389802705</v>
+        <v>0.009315810103514073</v>
       </c>
       <c r="E8" t="n">
-        <v>1.020506938783913</v>
+        <v>1.021492514417171</v>
       </c>
       <c r="F8" t="n">
-        <v>3.711773401229563</v>
+        <v>3.700917946756286</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01215767839500173</v>
+        <v>0.01238249761667237</v>
       </c>
       <c r="H8" t="n">
-        <v>0.461186536628251</v>
+        <v>0.4499607392653746</v>
       </c>
     </row>
     <row r="9">
@@ -662,25 +662,25 @@
         <v>366.458793969849</v>
       </c>
       <c r="B9" t="n">
-        <v>65.63002705074464</v>
+        <v>63.63981237294671</v>
       </c>
       <c r="C9" t="n">
-        <v>1.073371889974012</v>
+        <v>1.07584451974104</v>
       </c>
       <c r="D9" t="n">
-        <v>0.007905154163493217</v>
+        <v>0.007990914779688763</v>
       </c>
       <c r="E9" t="n">
-        <v>1.020465299584839</v>
+        <v>1.021450477903403</v>
       </c>
       <c r="F9" t="n">
-        <v>3.41122294762535</v>
+        <v>3.403763872907331</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01223938573251972</v>
+        <v>0.01245742152454838</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4621574346218282</v>
+        <v>0.4509080045132614</v>
       </c>
     </row>
     <row r="10">
@@ -688,25 +688,25 @@
         <v>416.710050251256</v>
       </c>
       <c r="B10" t="n">
-        <v>81.18059487776932</v>
+        <v>78.98544298635835</v>
       </c>
       <c r="C10" t="n">
-        <v>1.080714116249677</v>
+        <v>1.083096300337208</v>
       </c>
       <c r="D10" t="n">
-        <v>0.006905584363850568</v>
+        <v>0.00698595224590323</v>
       </c>
       <c r="E10" t="n">
-        <v>1.020422370078327</v>
+        <v>1.021407146838909</v>
       </c>
       <c r="F10" t="n">
-        <v>3.146424455453224</v>
+        <v>3.140733433858109</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01232603045592737</v>
+        <v>0.01253672791150673</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4631354784896018</v>
+        <v>0.4518622416967553</v>
       </c>
     </row>
     <row r="11">
@@ -714,25 +714,25 @@
         <v>466.961306532663</v>
       </c>
       <c r="B11" t="n">
-        <v>97.28549108130369</v>
+        <v>94.92764703619653</v>
       </c>
       <c r="C11" t="n">
-        <v>1.088318069583584</v>
+        <v>1.090629999596705</v>
       </c>
       <c r="D11" t="n">
-        <v>0.006121502253461602</v>
+        <v>0.006197662737811115</v>
       </c>
       <c r="E11" t="n">
-        <v>1.020378150264379</v>
+        <v>1.021362521223687</v>
       </c>
       <c r="F11" t="n">
-        <v>2.914577231597181</v>
+        <v>2.909641213845917</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01241752172498829</v>
+        <v>0.01262030528713326</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4641206682315723</v>
+        <v>0.4528234508158562</v>
       </c>
     </row>
     <row r="12">
@@ -740,25 +740,25 @@
         <v>517.21256281407</v>
       </c>
       <c r="B12" t="n">
-        <v>113.8055240997407</v>
+        <v>111.3245981602331</v>
       </c>
       <c r="C12" t="n">
-        <v>1.096118030450096</v>
+        <v>1.098378595597294</v>
       </c>
       <c r="D12" t="n">
-        <v>0.005490129454935887</v>
+        <v>0.005562917604361999</v>
       </c>
       <c r="E12" t="n">
-        <v>1.020332640142992</v>
+        <v>1.021316601057738</v>
       </c>
       <c r="F12" t="n">
-        <v>2.711810415185508</v>
+        <v>2.707022244419986</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01251381093720314</v>
+        <v>0.01270808111083593</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4651130038477391</v>
+        <v>0.4537916318705641</v>
       </c>
     </row>
     <row r="13">
@@ -766,25 +766,25 @@
         <v>567.463819095477</v>
       </c>
       <c r="B13" t="n">
-        <v>130.6345872962748</v>
+        <v>128.0673442522069</v>
       </c>
       <c r="C13" t="n">
-        <v>1.104063900425448</v>
+        <v>1.106290601580953</v>
       </c>
       <c r="D13" t="n">
-        <v>0.004970926288297838</v>
+        <v>0.005040950429199336</v>
       </c>
       <c r="E13" t="n">
-        <v>1.020285839714169</v>
+        <v>1.021269386341061</v>
       </c>
       <c r="F13" t="n">
-        <v>2.534165618852122</v>
+        <v>2.529176318278741</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01261487967926454</v>
+        <v>0.01280001052013846</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4661124853381028</v>
+        <v>0.4547667848608792</v>
       </c>
     </row>
     <row r="14">
@@ -792,25 +792,25 @@
         <v>617.715075376884</v>
       </c>
       <c r="B14" t="n">
-        <v>147.6906527639782</v>
+        <v>145.0710376385365</v>
       </c>
       <c r="C14" t="n">
-        <v>1.112116949897944</v>
+        <v>1.114325921657954</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004536546169726682</v>
+        <v>0.004604261155742565</v>
       </c>
       <c r="E14" t="n">
-        <v>1.020237748977908</v>
+        <v>1.021220877073657</v>
       </c>
       <c r="F14" t="n">
-        <v>2.378008031970626</v>
+        <v>2.372629242108838</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01272073156697052</v>
+        <v>0.01289606874691318</v>
       </c>
       <c r="H14" t="n">
-        <v>0.467119112702663</v>
+        <v>0.4557489097868012</v>
       </c>
     </row>
     <row r="15">
@@ -818,25 +818,25 @@
         <v>667.966331658292</v>
       </c>
       <c r="B15" t="n">
-        <v>164.9095400088511</v>
+        <v>162.2688158075273</v>
       </c>
       <c r="C15" t="n">
-        <v>1.120246875941373</v>
+        <v>1.122452959064555</v>
       </c>
       <c r="D15" t="n">
-        <v>0.004167873012219574</v>
+        <v>0.004233625910660917</v>
       </c>
       <c r="E15" t="n">
-        <v>1.02018836793421</v>
+        <v>1.021171073255527</v>
       </c>
       <c r="F15" t="n">
-        <v>2.240161855233584</v>
+        <v>2.234303430188285</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01283138639463601</v>
+        <v>0.01299624574141101</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4681328859414199</v>
+        <v>0.4567380066483304</v>
       </c>
     </row>
     <row r="16">
@@ -844,25 +844,25 @@
         <v>718.217587939699</v>
       </c>
       <c r="B16" t="n">
-        <v>182.2405151556376</v>
+        <v>179.6074486344044</v>
       </c>
       <c r="C16" t="n">
-        <v>1.128429724472762</v>
+        <v>1.130646559201661</v>
       </c>
       <c r="D16" t="n">
-        <v>0.003851141908932315</v>
+        <v>0.003915201691698098</v>
       </c>
       <c r="E16" t="n">
-        <v>1.020137696583075</v>
+        <v>1.021119974886668</v>
       </c>
       <c r="F16" t="n">
-        <v>2.117920640290055</v>
+        <v>2.111551390397616</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01294687571360622</v>
+        <v>0.0131005421791645</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4691538050543735</v>
+        <v>0.4577340754454666</v>
       </c>
     </row>
     <row r="17">
@@ -870,25 +870,25 @@
         <v>768.468844221106</v>
       </c>
       <c r="B17" t="n">
-        <v>199.6431235923621</v>
+        <v>197.0441858612375</v>
       </c>
       <c r="C17" t="n">
-        <v>1.136646394780272</v>
+        <v>1.138886519869782</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0035761894954473</v>
+        <v>0.003638767015901913</v>
       </c>
       <c r="E17" t="n">
-        <v>1.020085734924502</v>
+        <v>1.021067581967083</v>
       </c>
       <c r="F17" t="n">
-        <v>2.009006333217672</v>
+        <v>2.002129561578709</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01306723932187674</v>
+        <v>0.01320896636568443</v>
       </c>
       <c r="H17" t="n">
-        <v>0.4701818700415235</v>
+        <v>0.4587371161782098</v>
       </c>
     </row>
     <row r="18">
@@ -896,25 +896,25 @@
         <v>818.720100502513</v>
       </c>
       <c r="B18" t="n">
-        <v>217.0848708405942</v>
+        <v>214.5444358176717</v>
       </c>
       <c r="C18" t="n">
-        <v>1.144881544542259</v>
+        <v>1.147156494317834</v>
       </c>
       <c r="D18" t="n">
-        <v>0.003335348628166013</v>
+        <v>0.003396610467845565</v>
       </c>
       <c r="E18" t="n">
-        <v>1.020032482958493</v>
+        <v>1.02101389449677</v>
       </c>
       <c r="F18" t="n">
-        <v>1.911511885668433</v>
+        <v>1.9041502489964</v>
       </c>
       <c r="G18" t="n">
-        <v>0.01319252234718118</v>
+        <v>0.01332153174142876</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4712170809028703</v>
+        <v>0.4597471288465601</v>
       </c>
     </row>
     <row r="19">
@@ -922,25 +922,25 @@
         <v>868.97135678392</v>
       </c>
       <c r="B19" t="n">
-        <v>234.5394979191014</v>
+        <v>232.0800303109158</v>
       </c>
       <c r="C19" t="n">
-        <v>1.153122775537377</v>
+        <v>1.155443171293965</v>
       </c>
       <c r="D19" t="n">
-        <v>0.003122726558265435</v>
+        <v>0.003182804877686854</v>
       </c>
       <c r="E19" t="n">
-        <v>1.019977940685045</v>
+        <v>1.02095891247573</v>
       </c>
       <c r="F19" t="n">
-        <v>1.823843047001256</v>
+        <v>1.816029257125665</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01332277272300646</v>
+        <v>0.01343825479863412</v>
       </c>
       <c r="H19" t="n">
-        <v>0.4722594376384137</v>
+        <v>0.4607641134505175</v>
       </c>
     </row>
     <row r="20">
@@ -948,25 +948,25 @@
         <v>919.222613065327</v>
       </c>
       <c r="B20" t="n">
-        <v>251.9856806969353</v>
+        <v>249.6279098506167</v>
       </c>
       <c r="C20" t="n">
-        <v>1.161360019541989</v>
+        <v>1.163735653731193</v>
       </c>
       <c r="D20" t="n">
-        <v>0.002933719847285821</v>
+        <v>0.002992719559479817</v>
       </c>
       <c r="E20" t="n">
-        <v>1.019922108104161</v>
+        <v>1.020902635903963</v>
       </c>
       <c r="F20" t="n">
-        <v>1.744665647065493</v>
+        <v>1.736436821755457</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01345803892903491</v>
+        <v>0.01355915328808227</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4733089402481536</v>
+        <v>0.4617880699900818</v>
       </c>
     </row>
     <row r="21">
@@ -974,25 +974,25 @@
         <v>969.473869346734</v>
       </c>
       <c r="B21" t="n">
-        <v>269.4060364906328</v>
+        <v>267.1691149725249</v>
       </c>
       <c r="C21" t="n">
-        <v>1.169585069293397</v>
+        <v>1.172024982084065</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002764680124861169</v>
+        <v>0.002822684232746949</v>
       </c>
       <c r="E21" t="n">
-        <v>1.019864985215839</v>
+        <v>1.020845064781469</v>
       </c>
       <c r="F21" t="n">
-        <v>1.672860318436076</v>
+        <v>1.664254609418042</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01359836791407656</v>
+        <v>0.0136842446361167</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4743655887320903</v>
+        <v>0.4628189984652533</v>
       </c>
     </row>
     <row r="22">
@@ -1000,25 +1000,25 @@
         <v>1019.72512562814</v>
       </c>
       <c r="B22" t="n">
-        <v>286.786356567369</v>
+        <v>284.6880036440954</v>
       </c>
       <c r="C22" t="n">
-        <v>1.177791216114938</v>
+        <v>1.180303764503335</v>
       </c>
       <c r="D22" t="n">
-        <v>0.002612678653924532</v>
+        <v>0.002669752303253037</v>
       </c>
       <c r="E22" t="n">
-        <v>1.019806572020081</v>
+        <v>1.020786199108247</v>
       </c>
       <c r="F22" t="n">
-        <v>1.607484668403681</v>
+        <v>1.59853930782673</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0137438031511512</v>
+        <v>0.0138135445201217</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4754293830902234</v>
+        <v>0.4638568988760317</v>
       </c>
     </row>
     <row r="23">
@@ -1026,25 +1026,25 @@
         <v>1069.97638190955</v>
       </c>
       <c r="B23" t="n">
-        <v>304.1150069690437</v>
+        <v>302.171637829021</v>
       </c>
       <c r="C23" t="n">
-        <v>1.185972967014084</v>
+        <v>1.188565886948921</v>
       </c>
       <c r="D23" t="n">
-        <v>0.002475337219555233</v>
+        <v>0.002531530838288923</v>
       </c>
       <c r="E23" t="n">
-        <v>1.019746868516885</v>
+        <v>1.020726038884298</v>
       </c>
       <c r="F23" t="n">
-        <v>1.547742138727972</v>
+        <v>1.53849236586994</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01389438279683529</v>
+        <v>0.0139470655697604</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4765003233225533</v>
+        <v>0.4649017712224172</v>
       </c>
     </row>
     <row r="24">
@@ -1052,25 +1052,25 @@
         <v>1120.22763819095</v>
       </c>
       <c r="B24" t="n">
-        <v>321.3824562831662</v>
+        <v>319.609298132176</v>
       </c>
       <c r="C24" t="n">
-        <v>1.194125821718691</v>
+        <v>1.196806283828959</v>
       </c>
       <c r="D24" t="n">
-        <v>0.002350704515465536</v>
+        <v>0.00240605629425009</v>
       </c>
       <c r="E24" t="n">
-        <v>1.019685874706251</v>
+        <v>1.020664584109622</v>
       </c>
       <c r="F24" t="n">
-        <v>1.49295656387156</v>
+        <v>1.483435094120562</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01405013794359537</v>
+        <v>0.01408481617472417</v>
       </c>
       <c r="H24" t="n">
-        <v>0.4775784094290796</v>
+        <v>0.4659536155044097</v>
       </c>
     </row>
     <row r="25">
@@ -1078,25 +1078,25 @@
         <v>1170.47889447236</v>
       </c>
       <c r="B25" t="n">
-        <v>338.580900227564</v>
+        <v>336.9920964859089</v>
       </c>
       <c r="C25" t="n">
-        <v>1.202246095424045</v>
+        <v>1.205020754969593</v>
       </c>
       <c r="D25" t="n">
-        <v>0.00223716435558392</v>
+        <v>0.002291702247357422</v>
       </c>
       <c r="E25" t="n">
-        <v>1.019623590588181</v>
+        <v>1.020601834784218</v>
       </c>
       <c r="F25" t="n">
-        <v>1.442551451979095</v>
+        <v>1.43278827555655</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01421109096644987</v>
+        <v>0.01422679938944783</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4786636414098028</v>
+        <v>0.4670124317220093</v>
       </c>
     </row>
     <row r="26">
@@ -1104,25 +1104,25 @@
         <v>1220.73015075377</v>
       </c>
       <c r="B26" t="n">
-        <v>355.7039608267574</v>
+        <v>354.3126646410506</v>
       </c>
       <c r="C26" t="n">
-        <v>1.210330776758493</v>
+        <v>1.213205818407279</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002133366541489005</v>
+        <v>0.002187109906540602</v>
       </c>
       <c r="E26" t="n">
-        <v>1.019560016162673</v>
+        <v>1.020537790908088</v>
       </c>
       <c r="F26" t="n">
-        <v>1.396033120808503</v>
+        <v>1.386055497560793</v>
       </c>
       <c r="G26" t="n">
-        <v>0.01437725397495037</v>
+        <v>0.01437301193230486</v>
       </c>
       <c r="H26" t="n">
-        <v>0.4797560192647226</v>
+        <v>0.468078219875216</v>
       </c>
     </row>
     <row r="27">
@@ -1130,25 +1130,25 @@
         <v>1270.98140703518</v>
       </c>
       <c r="B27" t="n">
-        <v>372.7464436018859</v>
+        <v>371.5649018149281</v>
       </c>
       <c r="C27" t="n">
-        <v>1.218377413140263</v>
+        <v>1.221358591136519</v>
       </c>
       <c r="D27" t="n">
-        <v>0.002038174117359737</v>
+        <v>0.002091135104399756</v>
       </c>
       <c r="E27" t="n">
-        <v>1.019495151429727</v>
+        <v>1.02047245248123</v>
       </c>
       <c r="F27" t="n">
-        <v>1.352976954823758</v>
+        <v>1.342809521180751</v>
       </c>
       <c r="G27" t="n">
-        <v>0.014548627388672</v>
+        <v>0.01452344328188452</v>
       </c>
       <c r="H27" t="n">
-        <v>0.4808555429938389</v>
+        <v>0.4691509799640297</v>
       </c>
     </row>
     <row r="28">
@@ -1156,25 +1156,25 @@
         <v>1321.23266331658</v>
       </c>
       <c r="B28" t="n">
-        <v>389.7041402737947</v>
+        <v>388.743768901424</v>
       </c>
       <c r="C28" t="n">
-        <v>1.226384017623405</v>
+        <v>1.229476691861107</v>
       </c>
       <c r="D28" t="n">
-        <v>0.001950622652049373</v>
+        <v>0.002002807380596998</v>
       </c>
       <c r="E28" t="n">
-        <v>1.019428996389345</v>
+        <v>1.020405819503645</v>
       </c>
       <c r="F28" t="n">
-        <v>1.313016179714397</v>
+        <v>1.302681115430603</v>
       </c>
       <c r="G28" t="n">
-        <v>0.01472519865936304</v>
+        <v>0.01467807487645781</v>
       </c>
       <c r="H28" t="n">
-        <v>0.4819622125971517</v>
+        <v>0.4702307119884503</v>
       </c>
     </row>
     <row r="29">
@@ -1182,25 +1182,25 @@
         <v>1371.48391959799</v>
       </c>
       <c r="B29" t="n">
-        <v>406.5736674602999</v>
+        <v>405.8451196215274</v>
       </c>
       <c r="C29" t="n">
-        <v>1.234348992738433</v>
+        <v>1.237558161202088</v>
       </c>
       <c r="D29" t="n">
-        <v>0.001869888466645439</v>
+        <v>0.001921298057823369</v>
       </c>
       <c r="E29" t="n">
-        <v>1.019361551041525</v>
+        <v>1.020337891975332</v>
       </c>
       <c r="F29" t="n">
-        <v>1.275832665182959</v>
+        <v>1.26534988748284</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01490694116568986</v>
+        <v>0.01483687942490533</v>
       </c>
       <c r="H29" t="n">
-        <v>0.4830760280746614</v>
+        <v>0.4713174159484783</v>
       </c>
     </row>
     <row r="30">
@@ -1208,25 +1208,25 @@
         <v>1421.7351758794</v>
       </c>
       <c r="B30" t="n">
-        <v>423.3523340519781</v>
+        <v>422.8655611973151</v>
       </c>
       <c r="C30" t="n">
-        <v>1.24227106787359</v>
+        <v>1.245601395857406</v>
       </c>
       <c r="D30" t="n">
-        <v>0.001795263597791154</v>
+        <v>0.001845895087232201</v>
       </c>
       <c r="E30" t="n">
-        <v>1.019292815386268</v>
+        <v>1.020268669896292</v>
       </c>
       <c r="F30" t="n">
-        <v>1.241149363016292</v>
+        <v>1.230536728475274</v>
       </c>
       <c r="G30" t="n">
-        <v>0.01509381330711536</v>
+        <v>0.01499982033835329</v>
       </c>
       <c r="H30" t="n">
-        <v>0.4841969894263676</v>
+        <v>0.4724110918441131</v>
       </c>
     </row>
     <row r="31">
@@ -1234,25 +1234,25 @@
         <v>1471.9864321608</v>
       </c>
       <c r="B31" t="n">
-        <v>440.0380315962379</v>
+        <v>439.8023387836985</v>
       </c>
       <c r="C31" t="n">
-        <v>1.250149247519504</v>
+        <v>1.2536050939886</v>
       </c>
       <c r="D31" t="n">
-        <v>0.001726135890956238</v>
+        <v>0.001775983047552034</v>
       </c>
       <c r="E31" t="n">
-        <v>1.019222789423574</v>
+        <v>1.020198153266525</v>
       </c>
       <c r="F31" t="n">
-        <v>1.208724066057733</v>
+        <v>1.197997568615669</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0152857578218892</v>
+        <v>0.0151668512916591</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4853250966522703</v>
+        <v>0.4735117396753549</v>
       </c>
     </row>
     <row r="32">
@@ -1260,25 +1260,25 @@
         <v>1522.23768844221</v>
       </c>
       <c r="B32" t="n">
-        <v>456.629143259521</v>
+        <v>456.6532391404499</v>
       </c>
       <c r="C32" t="n">
-        <v>1.257982768285541</v>
+        <v>1.261568209699742</v>
       </c>
       <c r="D32" t="n">
-        <v>0.001661973042191832</v>
+        <v>0.001711027108918231</v>
       </c>
       <c r="E32" t="n">
-        <v>1.019151473153443</v>
+        <v>1.020126342086031</v>
       </c>
       <c r="F32" t="n">
-        <v>1.17834423696178</v>
+        <v>1.167518195562935</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01548270135047705</v>
+        <v>0.01533791592280655</v>
       </c>
       <c r="H32" t="n">
-        <v>0.4864603497523698</v>
+        <v>0.4746193594422038</v>
       </c>
     </row>
     <row r="33">
@@ -1286,25 +1286,25 @@
         <v>1572.48894472362</v>
       </c>
       <c r="B33" t="n">
-        <v>473.1244678806243</v>
+        <v>473.4165099790146</v>
       </c>
       <c r="C33" t="n">
-        <v>1.265771063041454</v>
+        <v>1.269489914923714</v>
       </c>
       <c r="D33" t="n">
-        <v>0.001602309709030811</v>
+        <v>0.001650560076460933</v>
       </c>
       <c r="E33" t="n">
-        <v>1.019078866575874</v>
+        <v>1.02005323635481</v>
       </c>
       <c r="F33" t="n">
-        <v>1.149822706093982</v>
+        <v>1.138909938643427</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01568455426021848</v>
+        <v>0.01551294767632841</v>
       </c>
       <c r="H33" t="n">
-        <v>0.4876027487266659</v>
+        <v>0.4757339511446599</v>
       </c>
     </row>
     <row r="34">
@@ -1312,25 +1312,25 @@
         <v>1622.74020100503</v>
       </c>
       <c r="B34" t="n">
-        <v>489.5231563514806</v>
+        <v>490.0907921506831</v>
       </c>
       <c r="C34" t="n">
-        <v>1.273513730879469</v>
+        <v>1.277369567376827</v>
       </c>
       <c r="D34" t="n">
-        <v>0.001546737028928873</v>
+        <v>0.001594171847883228</v>
       </c>
       <c r="E34" t="n">
-        <v>1.019004969690868</v>
+        <v>1.019978836072861</v>
       </c>
       <c r="F34" t="n">
-        <v>1.122994078036647</v>
+        <v>1.112006060339141</v>
       </c>
       <c r="G34" t="n">
-        <v>0.01589121073989722</v>
+        <v>0.01569186979422392</v>
       </c>
       <c r="H34" t="n">
-        <v>0.4887522935751586</v>
+        <v>0.4768555147827229</v>
       </c>
     </row>
     <row r="35">
@@ -1338,25 +1338,25 @@
         <v>1672.99145728643</v>
       </c>
       <c r="B35" t="n">
-        <v>505.8246581205732</v>
+        <v>506.6750624097407</v>
       </c>
       <c r="C35" t="n">
-        <v>1.281210511855778</v>
+        <v>1.285206683510792</v>
       </c>
       <c r="D35" t="n">
-        <v>0.001494894042325234</v>
+        <v>0.001541500779130312</v>
       </c>
       <c r="E35" t="n">
-        <v>1.018929782498425</v>
+        <v>1.019903141240185</v>
       </c>
       <c r="F35" t="n">
-        <v>1.097711717952195</v>
+        <v>1.086658727494093</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0161025491646801</v>
+        <v>0.01587459545463961</v>
       </c>
       <c r="H35" t="n">
-        <v>0.4899089842978478</v>
+        <v>0.477984050356393</v>
       </c>
     </row>
     <row r="36">
@@ -1364,25 +1364,25 @@
         <v>1723.24271356784</v>
       </c>
       <c r="B36" t="n">
-        <v>522.0286760493575</v>
+        <v>523.1685849279124</v>
       </c>
       <c r="C36" t="n">
-        <v>1.288861265675925</v>
+        <v>1.293000915600232</v>
       </c>
       <c r="D36" t="n">
-        <v>0.001446460634260494</v>
+        <v>0.001492226570085811</v>
       </c>
       <c r="E36" t="n">
-        <v>1.018853304998544</v>
+        <v>1.019826151856782</v>
       </c>
       <c r="F36" t="n">
-        <v>1.073845214258359</v>
+        <v>1.062736459388073</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0163184327230868</v>
+        <v>0.01606102805505027</v>
       </c>
       <c r="H36" t="n">
-        <v>0.4910728208947338</v>
+        <v>0.4791195578656701</v>
       </c>
     </row>
     <row r="37">
@@ -1390,25 +1390,25 @@
         <v>1773.49396984925</v>
       </c>
       <c r="B37" t="n">
-        <v>538.1351281930906</v>
+        <v>539.5708700841592</v>
       </c>
       <c r="C37" t="n">
-        <v>1.296465953649566</v>
+        <v>1.300752032268251</v>
       </c>
       <c r="D37" t="n">
-        <v>0.001401151695398527</v>
+        <v>0.001446064369954461</v>
       </c>
       <c r="E37" t="n">
-        <v>1.018775537191227</v>
+        <v>1.019747867922652</v>
       </c>
       <c r="F37" t="n">
-        <v>1.051278234071518</v>
+        <v>1.040121969511961</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01653871028889571</v>
+        <v>0.01625106163302181</v>
       </c>
       <c r="H37" t="n">
-        <v>0.4922438033658164</v>
+        <v>0.4802620373105543</v>
       </c>
     </row>
     <row r="38">
@@ -1416,25 +1416,25 @@
         <v>1823.74522613065</v>
       </c>
       <c r="B38" t="n">
-        <v>554.1441153466374</v>
+        <v>555.8816393290133</v>
       </c>
       <c r="C38" t="n">
-        <v>1.304024623367163</v>
+        <v>1.308459901882617</v>
       </c>
       <c r="D38" t="n">
-        <v>0.001358712268545818</v>
+        <v>0.001402759867906927</v>
       </c>
       <c r="E38" t="n">
-        <v>1.018696479076471</v>
+        <v>1.019668289437794</v>
       </c>
       <c r="F38" t="n">
-        <v>1.029906703779973</v>
+        <v>1.018710333585269</v>
       </c>
       <c r="G38" t="n">
-        <v>0.01676321751278715</v>
+        <v>0.01644458141409163</v>
       </c>
       <c r="H38" t="n">
-        <v>0.4934219317110954</v>
+        <v>0.4814114886910454</v>
       </c>
     </row>
     <row r="39">
@@ -1442,25 +1442,25 @@
         <v>1873.99648241206</v>
       </c>
       <c r="B39" t="n">
-        <v>570.0558934093681</v>
+        <v>572.100795141391</v>
       </c>
       <c r="C39" t="n">
-        <v>1.311537395652025</v>
+        <v>1.316124478358453</v>
       </c>
       <c r="D39" t="n">
-        <v>0.001318913496197644</v>
+        <v>0.001362085184535857</v>
       </c>
       <c r="E39" t="n">
-        <v>1.018616130654279</v>
+        <v>1.019587416402209</v>
       </c>
       <c r="F39" t="n">
-        <v>1.009637259789539</v>
+        <v>0.9984074289145043</v>
       </c>
       <c r="G39" t="n">
-        <v>0.01699177810163636</v>
+        <v>0.01664146447307535</v>
       </c>
       <c r="H39" t="n">
-        <v>0.4946072059305712</v>
+        <v>0.4825679120071437</v>
       </c>
     </row>
     <row r="40">
@@ -1468,25 +1468,25 @@
         <v>1924.24773869347</v>
       </c>
       <c r="B40" t="n">
-        <v>585.8708497937967</v>
+        <v>588.228395270944</v>
       </c>
       <c r="C40" t="n">
-        <v>1.319004453421611</v>
+        <v>1.32374578898612</v>
       </c>
       <c r="D40" t="n">
-        <v>0.001281549222447026</v>
+        <v>0.00132383541788137</v>
       </c>
       <c r="E40" t="n">
-        <v>1.01853449192465</v>
+        <v>1.019505248815897</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9903859246227684</v>
+        <v>0.9791286002563773</v>
       </c>
       <c r="G40" t="n">
-        <v>0.01722420524811955</v>
+        <v>0.01684158049239173</v>
       </c>
       <c r="H40" t="n">
-        <v>0.4957996260242437</v>
+        <v>0.4837313072588491</v>
       </c>
     </row>
     <row r="41">
@@ -1494,25 +1494,25 @@
         <v>1974.49899497487</v>
       </c>
       <c r="B41" t="n">
-        <v>601.5894832395526</v>
+        <v>604.2646305999322</v>
       </c>
       <c r="C41" t="n">
-        <v>1.326426032156659</v>
+        <v>1.331323923969554</v>
       </c>
       <c r="D41" t="n">
-        <v>0.001246433131769221</v>
+        <v>0.001287825727240425</v>
       </c>
       <c r="E41" t="n">
-        <v>1.018451562887583</v>
+        <v>1.019421786678858</v>
       </c>
       <c r="F41" t="n">
-        <v>0.9720769716859319</v>
+        <v>0.960797515440889</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0174603031700186</v>
+        <v>0.01704479259894126</v>
       </c>
       <c r="H41" t="n">
-        <v>0.4969991919921126</v>
+        <v>0.4849016744461613</v>
       </c>
     </row>
     <row r="42">
@@ -1520,25 +1520,25 @@
         <v>2024.75025125628</v>
       </c>
       <c r="B42" t="n">
-        <v>617.2123865047208</v>
+        <v>620.2098060724695</v>
       </c>
       <c r="C42" t="n">
-        <v>1.33380241172888</v>
+        <v>1.338859027414125</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00121339632993217</v>
+        <v>0.001253888860867351</v>
       </c>
       <c r="E42" t="n">
-        <v>1.018367343543079</v>
+        <v>1.019337029991091</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9546419485636977</v>
+        <v>0.9433451805334737</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01769986871738485</v>
+        <v>0.01725095825977034</v>
       </c>
       <c r="H42" t="n">
-        <v>0.4982059038341784</v>
+        <v>0.4860790135690808</v>
       </c>
     </row>
     <row r="43">
@@ -1546,25 +1546,25 @@
         <v>2075.00150753769</v>
       </c>
       <c r="B43" t="n">
-        <v>632.7402314960931</v>
+        <v>636.0643242315692</v>
       </c>
       <c r="C43" t="n">
-        <v>1.341133909380174</v>
+        <v>1.346351289546857</v>
       </c>
       <c r="D43" t="n">
-        <v>0.00118228529016872</v>
+        <v>0.001221873051605641</v>
       </c>
       <c r="E43" t="n">
-        <v>1.018281833891137</v>
+        <v>1.019250978752597</v>
       </c>
       <c r="F43" t="n">
-        <v>0.9380188339883555</v>
+        <v>0.926709089593026</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01794269300651859</v>
+        <v>0.01745993021624744</v>
       </c>
       <c r="H43" t="n">
-        <v>0.4994197615504407</v>
+        <v>0.4872633246276073</v>
       </c>
     </row>
     <row r="44">
@@ -1572,25 +1572,25 @@
         <v>2125.2527638191</v>
       </c>
       <c r="B44" t="n">
-        <v>648.1737564729767</v>
+        <v>651.828670980047</v>
       </c>
       <c r="C44" t="n">
-        <v>1.348420873680891</v>
+        <v>1.353800939987547</v>
       </c>
       <c r="D44" t="n">
-        <v>0.00115296010194937</v>
+        <v>0.001191640218648314</v>
       </c>
       <c r="E44" t="n">
-        <v>1.018195033931759</v>
+        <v>1.019163632963376</v>
       </c>
       <c r="F44" t="n">
-        <v>0.9221513079153992</v>
+        <v>0.9108324883663076</v>
       </c>
       <c r="G44" t="n">
-        <v>0.01818856304232276</v>
+        <v>0.01767155743675606</v>
       </c>
       <c r="H44" t="n">
-        <v>0.5006407651408996</v>
+        <v>0.4884546076217409</v>
       </c>
     </row>
     <row r="45">
@@ -1598,25 +1598,25 @@
         <v>2175.5040201005</v>
       </c>
       <c r="B45" t="n">
-        <v>663.5137550187769</v>
+        <v>667.5034032432422</v>
       </c>
       <c r="C45" t="n">
-        <v>1.355663679322747</v>
+        <v>1.361208241918627</v>
       </c>
       <c r="D45" t="n">
-        <v>0.001125292971076497</v>
+        <v>0.001163064424886454</v>
       </c>
       <c r="E45" t="n">
-        <v>1.018106943664943</v>
+        <v>1.019074992623427</v>
       </c>
       <c r="F45" t="n">
-        <v>0.9069881176230756</v>
+        <v>0.8956637347480463</v>
       </c>
       <c r="G45" t="n">
-        <v>0.01843726329464759</v>
+        <v>0.01788568606890149</v>
       </c>
       <c r="H45" t="n">
-        <v>0.501868914605555</v>
+        <v>0.4896528625514813</v>
       </c>
     </row>
     <row r="46">
@@ -1624,25 +1624,25 @@
         <v>2225.75527638191</v>
       </c>
       <c r="B46" t="n">
-        <v>678.7610665237275</v>
+        <v>683.0891382626021</v>
       </c>
       <c r="C46" t="n">
-        <v>1.362862722625227</v>
+        <v>1.368573487025702</v>
       </c>
       <c r="D46" t="n">
-        <v>0.001099166929012319</v>
+        <v>0.001136030548329914</v>
       </c>
       <c r="E46" t="n">
-        <v>1.01801756309069</v>
+        <v>1.018985057732752</v>
       </c>
       <c r="F46" t="n">
-        <v>0.8924825255987734</v>
+        <v>0.8811557416869792</v>
       </c>
       <c r="G46" t="n">
-        <v>0.01868857719939889</v>
+        <v>0.01810216037383365</v>
       </c>
       <c r="H46" t="n">
-        <v>0.5031042099444073</v>
+        <v>0.490858089416829</v>
       </c>
     </row>
     <row r="47">
@@ -1650,25 +1650,25 @@
         <v>2276.00653266332</v>
       </c>
       <c r="B47" t="n">
-        <v>693.9165679625551</v>
+        <v>698.5865442912991</v>
       </c>
       <c r="C47" t="n">
-        <v>1.370018417653396</v>
+        <v>1.375896991100642</v>
       </c>
       <c r="D47" t="n">
-        <v>0.001074474716836002</v>
+        <v>0.001110433133366147</v>
       </c>
       <c r="E47" t="n">
-        <v>1.017926892208999</v>
+        <v>1.018893828291349</v>
       </c>
       <c r="F47" t="n">
-        <v>0.8785918273061044</v>
+        <v>0.8672654905559048</v>
       </c>
       <c r="G47" t="n">
-        <v>0.0189422885609173</v>
+        <v>0.01832082362736653</v>
       </c>
       <c r="H47" t="n">
-        <v>0.5043466511574561</v>
+        <v>0.4920702882177837</v>
       </c>
     </row>
     <row r="48">
@@ -1676,25 +1676,25 @@
         <v>2326.25778894472</v>
       </c>
       <c r="B48" t="n">
-        <v>708.9811667844475</v>
+        <v>713.9963324981362</v>
       </c>
       <c r="C48" t="n">
-        <v>1.377131192860887</v>
+        <v>1.383179090215665</v>
       </c>
       <c r="D48" t="n">
-        <v>0.001051117815340101</v>
+        <v>0.001086175393535482</v>
       </c>
       <c r="E48" t="n">
-        <v>1.017834931019872</v>
+        <v>1.018801304299219</v>
       </c>
       <c r="F48" t="n">
-        <v>0.865276928842577</v>
+        <v>0.8539536049271039</v>
       </c>
       <c r="G48" t="n">
-        <v>0.01919818283814416</v>
+        <v>0.01854151897498483</v>
       </c>
       <c r="H48" t="n">
-        <v>0.5055962382447013</v>
+        <v>0.4932894589543452</v>
       </c>
     </row>
     <row r="49">
@@ -1702,25 +1702,25 @@
         <v>2376.50904522613</v>
       </c>
       <c r="B49" t="n">
-        <v>723.9557947605264</v>
+        <v>729.3192499151149</v>
       </c>
       <c r="C49" t="n">
-        <v>1.384201488184972</v>
+        <v>1.390420137390619</v>
       </c>
       <c r="D49" t="n">
-        <v>0.001029005597803087</v>
+        <v>0.001063168342330804</v>
       </c>
       <c r="E49" t="n">
-        <v>1.017741679523307</v>
+        <v>1.018707485756361</v>
       </c>
       <c r="F49" t="n">
-        <v>0.8525019760783377</v>
+        <v>0.8411839762822327</v>
       </c>
       <c r="G49" t="n">
-        <v>0.01945604830289698</v>
+        <v>0.01876409023039852</v>
       </c>
       <c r="H49" t="n">
-        <v>0.5068529712061433</v>
+        <v>0.4945156016265139</v>
       </c>
     </row>
     <row r="50">
@@ -1728,25 +1728,25 @@
         <v>2426.76030150754</v>
       </c>
       <c r="B50" t="n">
-        <v>738.8414026572212</v>
+        <v>744.5560732883584</v>
       </c>
       <c r="C50" t="n">
-        <v>1.391229752531591</v>
+        <v>1.397620499687151</v>
       </c>
       <c r="D50" t="n">
-        <v>0.001008054586109141</v>
+        <v>0.001041330032490189</v>
       </c>
       <c r="E50" t="n">
-        <v>1.017647137719304</v>
+        <v>1.018612372662777</v>
       </c>
       <c r="F50" t="n">
-        <v>0.8402340281745659</v>
+        <v>0.8289234345007482</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0197156770639633</v>
+        <v>0.01898838260993222</v>
       </c>
       <c r="H50" t="n">
-        <v>0.5081168500417821</v>
+        <v>0.4957487162342898</v>
       </c>
     </row>
     <row r="51">
@@ -1754,25 +1754,25 @@
         <v>2477.01155778894</v>
       </c>
       <c r="B51" t="n">
-        <v>753.6389556235027</v>
+        <v>759.7076037126441</v>
       </c>
       <c r="C51" t="n">
-        <v>1.398216441597425</v>
+        <v>1.404780555673189</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0009881877942921511</v>
+        <v>0.001020584887516272</v>
       </c>
       <c r="E51" t="n">
-        <v>1.017551305607865</v>
+        <v>1.018515965018465</v>
       </c>
       <c r="F51" t="n">
-        <v>0.8284427694662143</v>
+        <v>0.8171414570633077</v>
       </c>
       <c r="G51" t="n">
-        <v>0.01997686595544607</v>
+        <v>0.0192142433975482</v>
       </c>
       <c r="H51" t="n">
-        <v>0.5093878747516172</v>
+        <v>0.4969888027776725</v>
       </c>
     </row>
     <row r="52">
@@ -1780,25 +1780,25 @@
         <v>2527.26281407035</v>
       </c>
       <c r="B52" t="n">
-        <v>768.3494291961605</v>
+        <v>774.774661946889</v>
       </c>
       <c r="C52" t="n">
-        <v>1.40516201598378</v>
+        <v>1.411900693209208</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0009693341463840578</v>
+        <v>0.001000863111852492</v>
       </c>
       <c r="E52" t="n">
-        <v>1.017454183188988</v>
+        <v>1.018418262823426</v>
       </c>
       <c r="F52" t="n">
-        <v>0.8171002545986827</v>
+        <v>0.8058099118172397</v>
       </c>
       <c r="G52" t="n">
-        <v>0.0202394172917366</v>
+        <v>0.01944152253764123</v>
       </c>
       <c r="H52" t="n">
-        <v>0.5106660453356492</v>
+        <v>0.4982358612566625</v>
       </c>
     </row>
     <row r="53">
@@ -1806,25 +1806,25 @@
         <v>2577.51407035176</v>
       </c>
       <c r="B53" t="n">
-        <v>782.9738058410715</v>
+        <v>789.7580843224423</v>
       </c>
       <c r="C53" t="n">
-        <v>1.412066939563541</v>
+        <v>1.418981307514641</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0009514279577508361</v>
+        <v>0.0009821001683798397</v>
       </c>
       <c r="E53" t="n">
-        <v>1.017355770462674</v>
+        <v>1.018319266077659</v>
       </c>
       <c r="F53" t="n">
-        <v>0.8061806825641102</v>
+        <v>0.7949028289124345</v>
       </c>
       <c r="G53" t="n">
-        <v>0.02050313949460859</v>
+        <v>0.01967007315481584</v>
       </c>
       <c r="H53" t="n">
-        <v>0.5119513617938777</v>
+        <v>0.4994898916712595</v>
       </c>
     </row>
     <row r="54">
@@ -1832,25 +1832,25 @@
         <v>2627.76532663317</v>
       </c>
       <c r="B54" t="n">
-        <v>797.5130719600932</v>
+        <v>804.6587191684036</v>
       </c>
       <c r="C54" t="n">
-        <v>1.418931678067973</v>
+        <v>1.42602279947862</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0009344084709869381</v>
+        <v>0.0009642363137495295</v>
       </c>
       <c r="E54" t="n">
-        <v>1.017256067428923</v>
+        <v>1.018218974781166</v>
       </c>
       <c r="F54" t="n">
-        <v>0.7956601959166818</v>
+        <v>0.7843961981542941</v>
       </c>
       <c r="G54" t="n">
-        <v>0.02076784760023433</v>
+        <v>0.01989975200162622</v>
       </c>
       <c r="H54" t="n">
-        <v>0.5132438241263029</v>
+        <v>0.5007508940214636</v>
       </c>
     </row>
     <row r="55">
@@ -1858,25 +1858,25 @@
         <v>2678.01658291457</v>
       </c>
       <c r="B55" t="n">
-        <v>811.968215302948</v>
+        <v>819.4774236884921</v>
       </c>
       <c r="C55" t="n">
-        <v>1.425756697864741</v>
+        <v>1.433025574184093</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0009182194389820555</v>
+        <v>0.0009472161836037578</v>
       </c>
       <c r="E55" t="n">
-        <v>1.017155074087734</v>
+        <v>1.018117388933945</v>
       </c>
       <c r="F55" t="n">
-        <v>0.7855167019792395</v>
+        <v>0.7742677885573468</v>
       </c>
       <c r="G55" t="n">
-        <v>0.02103336365547901</v>
+        <v>0.02013041983670107</v>
       </c>
       <c r="H55" t="n">
-        <v>0.5145434323329244</v>
+        <v>0.5020188683072744</v>
       </c>
     </row>
     <row r="56">
@@ -1884,25 +1884,25 @@
         <v>2728.26783919598</v>
       </c>
       <c r="B56" t="n">
-        <v>826.3402227318994</v>
+        <v>834.2150612329443</v>
       </c>
       <c r="C56" t="n">
-        <v>1.43254246490249</v>
+        <v>1.439990039618625</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0009028087490312579</v>
+        <v>0.0009309884210120035</v>
       </c>
       <c r="E56" t="n">
-        <v>1.017052790439109</v>
+        <v>1.018014508535997</v>
       </c>
       <c r="F56" t="n">
-        <v>0.7757297133026748</v>
+        <v>0.7644969873358831</v>
       </c>
       <c r="G56" t="n">
-        <v>0.02129951701373281</v>
+        <v>0.0203619417367959</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5158501864137429</v>
+        <v>0.5032938145286926</v>
       </c>
     </row>
     <row r="57">
@@ -1910,25 +1910,25 @@
         <v>2778.51909547739</v>
       </c>
       <c r="B57" t="n">
-        <v>840.6300782940403</v>
+        <v>848.8724989164061</v>
       </c>
       <c r="C57" t="n">
-        <v>1.43928944380068</v>
+        <v>1.446916605548707</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0008881280828818477</v>
+        <v>0.0009155053425087591</v>
       </c>
       <c r="E57" t="n">
-        <v>1.016949216483046</v>
+        <v>1.017910333587321</v>
       </c>
       <c r="F57" t="n">
-        <v>0.7662802050194875</v>
+        <v>0.7550646559510158</v>
       </c>
       <c r="G57" t="n">
-        <v>0.02156614454089364</v>
+        <v>0.02059418734712522</v>
       </c>
       <c r="H57" t="n">
-        <v>0.517164086368758</v>
+        <v>0.5045757326857178</v>
       </c>
     </row>
     <row r="58">
@@ -1936,25 +1936,25 @@
         <v>2828.77035175879</v>
       </c>
       <c r="B58" t="n">
-        <v>854.8387615621946</v>
+        <v>863.4506055393332</v>
       </c>
       <c r="C58" t="n">
-        <v>1.445998097066238</v>
+        <v>1.453805682537476</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0008741326084388082</v>
+        <v>0.0009007226369964184</v>
       </c>
       <c r="E58" t="n">
-        <v>1.016844352219545</v>
+        <v>1.017804864087918</v>
       </c>
       <c r="F58" t="n">
-        <v>0.757150487054898</v>
+        <v>0.745953001158323</v>
       </c>
       <c r="G58" t="n">
-        <v>0.02183309074204898</v>
+        <v>0.02082703107486304</v>
       </c>
       <c r="H58" t="n">
-        <v>0.5184851321979693</v>
+        <v>0.5058646227783496</v>
       </c>
     </row>
     <row r="59">
@@ -1962,25 +1962,25 @@
         <v>2879.0216080402</v>
       </c>
       <c r="B59" t="n">
-        <v>868.967246210529</v>
+        <v>877.9502497759009</v>
       </c>
       <c r="C59" t="n">
-        <v>1.452668884421029</v>
+        <v>1.460657681088398</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0008607806995235396</v>
+        <v>0.0008865990935054661</v>
       </c>
       <c r="E59" t="n">
-        <v>1.016738197648608</v>
+        <v>1.017698100037789</v>
       </c>
       <c r="F59" t="n">
-        <v>0.7483240894327651</v>
+        <v>0.7371454592764828</v>
       </c>
       <c r="G59" t="n">
-        <v>0.02210020781899412</v>
+        <v>0.0210603522309882</v>
       </c>
       <c r="H59" t="n">
-        <v>0.5198133239013776</v>
+        <v>0.5071604848065889</v>
       </c>
     </row>
     <row r="60">
@@ -1988,25 +1988,25 @@
         <v>2929.27286432161</v>
       </c>
       <c r="B60" t="n">
-        <v>883.0164987954241</v>
+        <v>892.3722985961759</v>
       </c>
       <c r="C60" t="n">
-        <v>1.459302262226245</v>
+        <v>1.467473010899637</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0008480336806241946</v>
+        <v>0.0008730963544075567</v>
       </c>
       <c r="E60" t="n">
-        <v>1.016630752770233</v>
+        <v>1.017590041436932</v>
       </c>
       <c r="F60" t="n">
-        <v>0.7397856591469449</v>
+        <v>0.7286265921327884</v>
       </c>
       <c r="G60" t="n">
-        <v>0.02236735566812226</v>
+        <v>0.02129403512574833</v>
       </c>
       <c r="H60" t="n">
-        <v>0.5211486614789825</v>
+        <v>0.5084633187704353</v>
       </c>
     </row>
     <row r="61">
@@ -2014,25 +2014,25 @@
         <v>2979.52412060302</v>
       </c>
       <c r="B61" t="n">
-        <v>896.987477716055</v>
+        <v>906.7176158944734</v>
       </c>
       <c r="C61" t="n">
-        <v>1.465898682991637</v>
+        <v>1.474252080215873</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0008358555940184679</v>
+        <v>0.0008601786911786251</v>
       </c>
       <c r="E61" t="n">
-        <v>1.016522017584421</v>
+        <v>1.017480688285347</v>
       </c>
       <c r="F61" t="n">
-        <v>0.7315208672681103</v>
+        <v>0.7203819933426506</v>
       </c>
       <c r="G61" t="n">
-        <v>0.02263440182745633</v>
+        <v>0.02152796912293553</v>
       </c>
       <c r="H61" t="n">
-        <v>0.5224911449307841</v>
+        <v>0.5097731246698887</v>
       </c>
     </row>
     <row r="62">
@@ -2040,25 +2040,25 @@
         <v>3029.77537688442</v>
       </c>
       <c r="B62" t="n">
-        <v>910.8811323323481</v>
+        <v>920.9870612992963</v>
       </c>
       <c r="C62" t="n">
-        <v>1.472458594959063</v>
+        <v>1.480995295265917</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0008242129870094656</v>
+        <v>0.0008478128002243557</v>
       </c>
       <c r="E62" t="n">
-        <v>1.016411992091172</v>
+        <v>1.017370040583036</v>
       </c>
       <c r="F62" t="n">
-        <v>0.7235163251269493</v>
+        <v>0.7123982037526819</v>
       </c>
       <c r="G62" t="n">
-        <v>0.02290122138076828</v>
+        <v>0.02176204865798374</v>
       </c>
       <c r="H62" t="n">
-        <v>0.5238407742567821</v>
+        <v>0.5110899025049489</v>
       </c>
     </row>
     <row r="63">
@@ -2066,25 +2066,25 @@
         <v>3080.02663316583</v>
       </c>
       <c r="B63" t="n">
-        <v>924.6984022208353</v>
+        <v>935.1814891433492</v>
       </c>
       <c r="C63" t="n">
-        <v>1.478982441751133</v>
+        <v>1.487703059775982</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0008130747173098738</v>
+        <v>0.0008359676166264214</v>
       </c>
       <c r="E63" t="n">
-        <v>1.016300676290485</v>
+        <v>1.017258098329997</v>
       </c>
       <c r="F63" t="n">
-        <v>0.7157595085613565</v>
+        <v>0.7046626350250143</v>
       </c>
       <c r="G63" t="n">
-        <v>0.02316769682588568</v>
+        <v>0.02199617322461069</v>
       </c>
       <c r="H63" t="n">
-        <v>0.5251975494569768</v>
+        <v>0.5124136522756164</v>
       </c>
     </row>
     <row r="64">
@@ -2092,25 +2092,25 @@
         <v>3130.27788944724</v>
       </c>
       <c r="B64" t="n">
-        <v>938.4402165513908</v>
+        <v>949.3017475747289</v>
       </c>
       <c r="C64" t="n">
-        <v>1.485470662076939</v>
+        <v>1.494375774549662</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0008024117748520752</v>
+        <v>0.0008246141439557773</v>
       </c>
       <c r="E64" t="n">
-        <v>1.016188070182361</v>
+        <v>1.017144861526231</v>
       </c>
       <c r="F64" t="n">
-        <v>0.7082386893414977</v>
+        <v>0.6971635004680306</v>
       </c>
       <c r="G64" t="n">
-        <v>0.02343371791346595</v>
+        <v>0.0222302473343895</v>
       </c>
       <c r="H64" t="n">
-        <v>0.5265614705313683</v>
+        <v>0.5137443739818909</v>
       </c>
     </row>
     <row r="65">
@@ -2118,25 +2118,25 @@
         <v>3180.52914572864</v>
       </c>
       <c r="B65" t="n">
-        <v>952.107493569983</v>
+        <v>963.3486777927787</v>
       </c>
       <c r="C65" t="n">
-        <v>1.491923689487829</v>
+        <v>1.501013837106828</v>
       </c>
       <c r="D65" t="n">
-        <v>0.0007921971185034863</v>
+        <v>0.0008137252985398128</v>
       </c>
       <c r="E65" t="n">
-        <v>1.0160741737668</v>
+        <v>1.017030330171737</v>
       </c>
       <c r="F65" t="n">
-        <v>0.7009428729955555</v>
+        <v>0.689889752328617</v>
       </c>
       <c r="G65" t="n">
-        <v>0.02369918146173786</v>
+        <v>0.02246418045326501</v>
       </c>
       <c r="H65" t="n">
-        <v>0.5279325374799561</v>
+        <v>0.5150820676237722</v>
       </c>
     </row>
     <row r="66">
@@ -2144,25 +2144,25 @@
         <v>3230.78040201005</v>
       </c>
       <c r="B66" t="n">
-        <v>965.7011401743632</v>
+        <v>977.323113393987</v>
       </c>
       <c r="C66" t="n">
-        <v>1.498341952177076</v>
+        <v>1.507617641374517</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0007824055263351813</v>
+        <v>0.0008032757667719373</v>
       </c>
       <c r="E66" t="n">
-        <v>1.015958987043801</v>
+        <v>1.016914504266517</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6938617423531797</v>
+        <v>0.6828310248562198</v>
       </c>
       <c r="G66" t="n">
-        <v>0.02396399115199951</v>
+        <v>0.02269788691864534</v>
       </c>
       <c r="H66" t="n">
-        <v>0.5293107503027407</v>
+        <v>0.5164267332012608</v>
       </c>
     </row>
     <row r="67">
@@ -2170,25 +2170,25 @@
         <v>3281.03165829146</v>
       </c>
       <c r="B67" t="n">
-        <v>979.2220515712543</v>
+        <v>991.2258798151265</v>
       </c>
       <c r="C67" t="n">
-        <v>1.504725872818011</v>
+        <v>1.51418757742379</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0007730134582349567</v>
+        <v>0.0007932418742221402</v>
       </c>
       <c r="E67" t="n">
-        <v>1.015842510013366</v>
+        <v>1.016797383810569</v>
       </c>
       <c r="F67" t="n">
-        <v>0.686985606205242</v>
+        <v>0.6759775825313519</v>
       </c>
       <c r="G67" t="n">
-        <v>0.02422805730901818</v>
+        <v>0.02293128584031726</v>
       </c>
       <c r="H67" t="n">
-        <v>0.530696108999722</v>
+        <v>0.5177783707143565</v>
       </c>
     </row>
     <row r="68">
@@ -2196,25 +2196,25 @@
         <v>3331.28291457286</v>
       </c>
       <c r="B68" t="n">
-        <v>992.6711110049979</v>
+        <v>1005.057793862348</v>
       </c>
       <c r="C68" t="n">
-        <v>1.511075868435908</v>
+        <v>1.520724031247189</v>
       </c>
       <c r="D68" t="n">
-        <v>0.0007639989297784498</v>
+        <v>0.000783601465450697</v>
       </c>
       <c r="E68" t="n">
-        <v>1.015724742675493</v>
+        <v>1.016678968803894</v>
       </c>
       <c r="F68" t="n">
-        <v>0.6803053525493689</v>
+        <v>0.6693202729227707</v>
       </c>
       <c r="G68" t="n">
-        <v>0.0244912966699098</v>
+        <v>0.02316430098807222</v>
       </c>
       <c r="H68" t="n">
-        <v>0.5320886135708996</v>
+        <v>0.519136980163059</v>
       </c>
     </row>
     <row r="69">
@@ -2222,25 +2222,25 @@
         <v>3381.53417085427</v>
       </c>
       <c r="B69" t="n">
-        <v>1006.049189548827</v>
+        <v>1018.819663316233</v>
       </c>
       <c r="C69" t="n">
-        <v>1.517392350309432</v>
+        <v>1.527227384572106</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0007553413963780719</v>
+        <v>0.0007743337935498896</v>
       </c>
       <c r="E69" t="n">
-        <v>1.015605685030183</v>
+        <v>1.016559259246491</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6738124059523684</v>
+        <v>0.6628504836998232</v>
       </c>
       <c r="G69" t="n">
-        <v>0.02475363214457389</v>
+        <v>0.02339686066858125</v>
       </c>
       <c r="H69" t="n">
-        <v>0.5334882640162741</v>
+        <v>0.5205025615473687</v>
       </c>
     </row>
     <row r="70">
@@ -2248,25 +2248,25 @@
         <v>3431.78542713568</v>
       </c>
       <c r="B70" t="n">
-        <v>1019.357145950953</v>
+        <v>1032.512286603982</v>
       </c>
       <c r="C70" t="n">
-        <v>1.523675723897971</v>
+        <v>1.533698014705869</v>
       </c>
       <c r="D70" t="n">
-        <v>0.0007470216468221265</v>
+        <v>0.0007654194185434039</v>
       </c>
       <c r="E70" t="n">
-        <v>1.015485337077435</v>
+        <v>1.016438255138362</v>
       </c>
       <c r="F70" t="n">
-        <v>0.6674986886144395</v>
+        <v>0.6565601033807413</v>
       </c>
       <c r="G70" t="n">
-        <v>0.02501499257033032</v>
+        <v>0.02362889759374319</v>
       </c>
       <c r="H70" t="n">
-        <v>0.5348950603358453</v>
+        <v>0.5218751148672855</v>
       </c>
     </row>
     <row r="71">
@@ -2274,25 +2274,25 @@
         <v>3482.03668341709</v>
       </c>
       <c r="B71" t="n">
-        <v>1032.595826528664</v>
+        <v>1046.136452530971</v>
       </c>
       <c r="C71" t="n">
-        <v>1.529926388791627</v>
+        <v>1.540136294408885</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0007390217053984557</v>
+        <v>0.0007568401138635642</v>
       </c>
       <c r="E71" t="n">
-        <v>1.015363698817251</v>
+        <v>1.016315956479505</v>
       </c>
       <c r="F71" t="n">
-        <v>0.6613565847669587</v>
+        <v>0.6504414854450704</v>
       </c>
       <c r="G71" t="n">
-        <v>0.02527531246302738</v>
+        <v>0.02386034874244275</v>
       </c>
       <c r="H71" t="n">
-        <v>0.536309002529613</v>
+        <v>0.5232546401228094</v>
       </c>
     </row>
     <row r="72">
@@ -2300,25 +2300,25 @@
         <v>3532.28793969849</v>
       </c>
       <c r="B72" t="n">
-        <v>1045.766065104368</v>
+        <v>1059.692940064787</v>
       </c>
       <c r="C72" t="n">
-        <v>1.536144738681029</v>
+        <v>1.546542591792584</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0007313247418697679</v>
+        <v>0.0007485787802051684</v>
       </c>
       <c r="E72" t="n">
-        <v>1.015240770249628</v>
+        <v>1.016192363269921</v>
       </c>
       <c r="F72" t="n">
-        <v>0.6553789080767632</v>
+        <v>0.6444874154799224</v>
       </c>
       <c r="G72" t="n">
-        <v>0.02553453176657073</v>
+        <v>0.02409115521739669</v>
       </c>
       <c r="H72" t="n">
-        <v>0.5377300905975771</v>
+        <v>0.52464113731394</v>
       </c>
     </row>
     <row r="73">
@@ -2326,25 +2326,25 @@
         <v>3582.5391959799</v>
       </c>
       <c r="B73" t="n">
-        <v>1058.868682978301</v>
+        <v>1073.18251816559</v>
       </c>
       <c r="C73" t="n">
-        <v>1.542331161344439</v>
+        <v>1.552917270239256</v>
       </c>
       <c r="D73" t="n">
-        <v>0.000723914988633084</v>
+        <v>0.0007406193661232653</v>
       </c>
       <c r="E73" t="n">
-        <v>1.015116551374569</v>
+        <v>1.016067475509609</v>
       </c>
       <c r="F73" t="n">
-        <v>0.6495588717658367</v>
+        <v>0.6386910810661515</v>
       </c>
       <c r="G73" t="n">
-        <v>0.02579259560254681</v>
+        <v>0.0243212620985391</v>
       </c>
       <c r="H73" t="n">
-        <v>0.5391583245397383</v>
+        <v>0.526034606440678</v>
       </c>
     </row>
     <row r="74">
@@ -2352,25 +2352,25 @@
         <v>3632.79045226131</v>
       </c>
       <c r="B74" t="n">
-        <v>1071.904488933113</v>
+        <v>1086.605945657407</v>
       </c>
       <c r="C74" t="n">
-        <v>1.54848603864992</v>
+        <v>1.559260688341223</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0007167776644547991</v>
+        <v>0.0007329467948026402</v>
       </c>
       <c r="E74" t="n">
-        <v>1.014991042192073</v>
+        <v>1.015941293198571</v>
       </c>
       <c r="F74" t="n">
-        <v>0.6438900611869983</v>
+        <v>0.6330460441424843</v>
       </c>
       <c r="G74" t="n">
-        <v>0.0260494540213691</v>
+        <v>0.02455061829419417</v>
       </c>
       <c r="H74" t="n">
-        <v>0.5405937043560959</v>
+        <v>0.5274350475030231</v>
       </c>
     </row>
     <row r="75">
@@ -2378,25 +2378,25 @@
         <v>3683.04170854271</v>
       </c>
       <c r="B75" t="n">
-        <v>1084.874279266287</v>
+        <v>1099.963971135555</v>
       </c>
       <c r="C75" t="n">
-        <v>1.554609746570644</v>
+        <v>1.5655731998571</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0007098989042256546</v>
+        <v>0.0007255468964801144</v>
       </c>
       <c r="E75" t="n">
-        <v>1.014864242702139</v>
+        <v>1.015813816336805</v>
       </c>
       <c r="F75" t="n">
-        <v>0.6383664086239573</v>
+        <v>0.6275462156137561</v>
       </c>
       <c r="G75" t="n">
-        <v>0.02630506175618619</v>
+        <v>0.02477917639111095</v>
       </c>
       <c r="H75" t="n">
-        <v>0.5420362300466498</v>
+        <v>0.5288424605009748</v>
       </c>
     </row>
     <row r="76">
@@ -2404,25 +2404,25 @@
         <v>3733.29296482412</v>
       </c>
       <c r="B76" t="n">
-        <v>1097.778837846676</v>
+        <v>1113.257332905929</v>
       </c>
       <c r="C76" t="n">
-        <v>1.560702655211583</v>
+        <v>1.571855153683096</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0007032656942290063</v>
+        <v>0.000718406346048215</v>
       </c>
       <c r="E76" t="n">
-        <v>1.014736152904768</v>
+        <v>1.015685044924312</v>
       </c>
       <c r="F76" t="n">
-        <v>0.63298217010869</v>
+        <v>0.6221858319941973</v>
       </c>
       <c r="G76" t="n">
-        <v>0.02655937798058715</v>
+        <v>0.02500689250428206</v>
       </c>
       <c r="H76" t="n">
-        <v>0.5434859016114008</v>
+        <v>0.5302568454345339</v>
       </c>
     </row>
     <row r="77">
@@ -2430,25 +2430,25 @@
         <v>3783.54422110553</v>
       </c>
       <c r="B77" t="n">
-        <v>1110.618936191884</v>
+        <v>1126.486758952308</v>
       </c>
       <c r="C77" t="n">
-        <v>1.566765128846049</v>
+        <v>1.578106893837568</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0006968658124592526</v>
+        <v>0.0007115126054113211</v>
       </c>
       <c r="E77" t="n">
-        <v>1.014606772799959</v>
+        <v>1.015554978961091</v>
       </c>
       <c r="F77" t="n">
-        <v>0.6277319040707542</v>
+        <v>0.6169594338986105</v>
       </c>
       <c r="G77" t="n">
-        <v>0.02681236607100285</v>
+        <v>0.02523372612733275</v>
       </c>
       <c r="H77" t="n">
-        <v>0.5449427190503483</v>
+        <v>0.5316782023037001</v>
       </c>
     </row>
     <row r="78">
@@ -2456,25 +2456,25 @@
         <v>3833.79547738693</v>
       </c>
       <c r="B78" t="n">
-        <v>1123.395333563688</v>
+        <v>1139.652966928366</v>
       </c>
       <c r="C78" t="n">
-        <v>1.572797525960744</v>
+        <v>1.584328759457248</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0006906877735677531</v>
+        <v>0.00070485387020333</v>
       </c>
       <c r="E78" t="n">
-        <v>1.014476102387714</v>
+        <v>1.015423618447144</v>
       </c>
       <c r="F78" t="n">
-        <v>0.6226104516522736</v>
+        <v>0.6118618462135844</v>
       </c>
       <c r="G78" t="n">
-        <v>0.02706399337455342</v>
+        <v>0.02545963998415629</v>
       </c>
       <c r="H78" t="n">
-        <v>0.5464066823634921</v>
+        <v>0.5331065311084731</v>
       </c>
     </row>
     <row r="79">
@@ -2482,25 +2482,25 @@
         <v>3884.04673366834</v>
       </c>
       <c r="B79" t="n">
-        <v>1136.108777078956</v>
+        <v>1152.75666417138</v>
       </c>
       <c r="C79" t="n">
-        <v>1.578800199308129</v>
+        <v>1.590521084803715</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0006847207780501912</v>
+        <v>0.0006984190205102794</v>
       </c>
       <c r="E79" t="n">
-        <v>1.014344141668031</v>
+        <v>1.015290963382469</v>
       </c>
       <c r="F79" t="n">
-        <v>0.6176129185393139</v>
+        <v>0.6068881597980549</v>
       </c>
       <c r="G79" t="n">
-        <v>0.0273142309829706</v>
+        <v>0.02568459988236853</v>
       </c>
       <c r="H79" t="n">
-        <v>0.5478777915508328</v>
+        <v>0.5345418318488532</v>
       </c>
     </row>
     <row r="80">
@@ -2508,25 +2508,25 @@
         <v>3934.29798994975</v>
       </c>
       <c r="B80" t="n">
-        <v>1148.760001833752</v>
+        <v>1165.798547734893</v>
       </c>
       <c r="C80" t="n">
-        <v>1.584773495965025</v>
+        <v>1.596684199278835</v>
       </c>
       <c r="D80" t="n">
-        <v>0.000678954665322806</v>
+        <v>0.0006921975752723423</v>
       </c>
       <c r="E80" t="n">
-        <v>1.014210890640911</v>
+        <v>1.015157013767067</v>
       </c>
       <c r="F80" t="n">
-        <v>0.6127346581754447</v>
+        <v>0.6020337145777386</v>
       </c>
       <c r="G80" t="n">
-        <v>0.02756305351311461</v>
+        <v>0.02590857456906983</v>
       </c>
       <c r="H80" t="n">
-        <v>0.5493560466123701</v>
+        <v>0.5359841045248405</v>
       </c>
     </row>
     <row r="81">
@@ -2534,25 +2534,25 @@
         <v>3984.54924623116</v>
       </c>
       <c r="B81" t="n">
-        <v>1161.349731038751</v>
+        <v>1178.779304438057</v>
       </c>
       <c r="C81" t="n">
-        <v>1.590717757396548</v>
+        <v>1.602818427448077</v>
       </c>
       <c r="D81" t="n">
-        <v>0.000673379870365647</v>
+        <v>0.0006861796500676339</v>
       </c>
       <c r="E81" t="n">
-        <v>1.014076349306354</v>
+        <v>1.015021769600938</v>
       </c>
       <c r="F81" t="n">
-        <v>0.6079712562365928</v>
+        <v>0.5972940839114106</v>
       </c>
       <c r="G81" t="n">
-        <v>0.02781043889450029</v>
+        <v>0.02613153558932787</v>
       </c>
       <c r="H81" t="n">
-        <v>0.5508414475481042</v>
+        <v>0.5374333491364348</v>
       </c>
     </row>
     <row r="82">
@@ -2560,25 +2560,25 @@
         <v>4034.80050251256</v>
       </c>
       <c r="B82" t="n">
-        <v>1173.878676164118</v>
+        <v>1191.699610929438</v>
       </c>
       <c r="C82" t="n">
-        <v>1.596633319524509</v>
+        <v>1.608924089070667</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0006679873836385159</v>
+        <v>0.0006803559180059236</v>
       </c>
       <c r="E82" t="n">
-        <v>1.013940517664359</v>
+        <v>1.014885230884081</v>
       </c>
       <c r="F82" t="n">
-        <v>0.6033185162582394</v>
+        <v>0.5926650601190833</v>
       </c>
       <c r="G82" t="n">
-        <v>0.02805636816417672</v>
+        <v>0.02635345714772411</v>
       </c>
       <c r="H82" t="n">
-        <v>0.5523339943580344</v>
+        <v>0.5388895656836359</v>
       </c>
     </row>
     <row r="83">
@@ -2586,25 +2586,25 @@
         <v>4085.05175879397</v>
       </c>
       <c r="B83" t="n">
-        <v>1186.347537092364</v>
+        <v>1204.56013376349</v>
       </c>
       <c r="C83" t="n">
-        <v>1.602520512799592</v>
+        <v>1.615001499135721</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0006627687140014699</v>
+        <v>0.0006747175734831471</v>
       </c>
       <c r="E83" t="n">
-        <v>1.013803395714927</v>
+        <v>1.014747397616497</v>
       </c>
       <c r="F83" t="n">
-        <v>0.5987724463165861</v>
+        <v>0.5881426410727705</v>
       </c>
       <c r="G83" t="n">
-        <v>0.02830082526919355</v>
+        <v>0.02657431597326245</v>
       </c>
       <c r="H83" t="n">
-        <v>0.5538336870421618</v>
+        <v>0.5403527541664445</v>
       </c>
     </row>
     <row r="84">
@@ -2612,25 +2612,25 @@
         <v>4135.30301507538</v>
       </c>
       <c r="B84" t="n">
-        <v>1198.757002277752</v>
+        <v>1217.361529487898</v>
       </c>
       <c r="C84" t="n">
-        <v>1.608379662276615</v>
+        <v>1.621050967903527</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0006577158543943648</v>
+        <v>0.0006692562985692765</v>
       </c>
       <c r="E84" t="n">
-        <v>1.013664983458058</v>
+        <v>1.014608269798186</v>
       </c>
       <c r="F84" t="n">
-        <v>0.594329246674778</v>
+        <v>0.5837230177601567</v>
       </c>
       <c r="G84" t="n">
-        <v>0.0285437968768437</v>
+        <v>0.02679409118786694</v>
       </c>
       <c r="H84" t="n">
-        <v>0.5553405256004857</v>
+        <v>0.5418229145848599</v>
       </c>
     </row>
     <row r="85">
@@ -2638,25 +2638,25 @@
         <v>4185.55427135678</v>
       </c>
       <c r="B85" t="n">
-        <v>1211.107748911102</v>
+        <v>1230.104444740424</v>
       </c>
       <c r="C85" t="n">
-        <v>1.61421108769234</v>
+        <v>1.627072800951308</v>
       </c>
       <c r="D85" t="n">
-        <v>0.0006528212500515152</v>
+        <v>0.0006639642318207995</v>
       </c>
       <c r="E85" t="n">
-        <v>1.013525280893752</v>
+        <v>1.014467847429148</v>
       </c>
       <c r="F85" t="n">
-        <v>0.5899852983137133</v>
+        <v>0.5794025627399193</v>
       </c>
       <c r="G85" t="n">
-        <v>0.02878527219279065</v>
+        <v>0.02701276417867053</v>
       </c>
       <c r="H85" t="n">
-        <v>0.5568545100330058</v>
+        <v>0.5433000469388821</v>
       </c>
     </row>
     <row r="86">
@@ -2664,25 +2664,25 @@
         <v>4235.80552763819</v>
       </c>
       <c r="B86" t="n">
-        <v>1223.400443088878</v>
+        <v>1242.78951635382</v>
       </c>
       <c r="C86" t="n">
-        <v>1.620015103545313</v>
+        <v>1.633067299222799</v>
       </c>
       <c r="D86" t="n">
-        <v>0.0006480777690468076</v>
+        <v>0.0006588339393269147</v>
       </c>
       <c r="E86" t="n">
-        <v>1.013384288022008</v>
+        <v>1.014326130509382</v>
       </c>
       <c r="F86" t="n">
-        <v>0.5857371522745327</v>
+        <v>0.5751778194151846</v>
       </c>
       <c r="G86" t="n">
-        <v>0.02902524278713482</v>
+        <v>0.02723031847424524</v>
       </c>
       <c r="H86" t="n">
-        <v>0.558375640339723</v>
+        <v>0.5447841512285118</v>
       </c>
     </row>
     <row r="87">
@@ -2690,25 +2690,25 @@
         <v>4286.0567839196</v>
       </c>
       <c r="B87" t="n">
-        <v>1235.635739985604</v>
+        <v>1255.417371467626</v>
       </c>
       <c r="C87" t="n">
-        <v>1.625792019177268</v>
+        <v>1.639034759081078</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0006434786749822704</v>
+        <v>0.0006538583878144722</v>
       </c>
       <c r="E87" t="n">
-        <v>1.013242004842827</v>
+        <v>1.014183119038889</v>
       </c>
       <c r="F87" t="n">
-        <v>0.5815815197466734</v>
+        <v>0.5710454920583775</v>
       </c>
       <c r="G87" t="n">
-        <v>0.02926370242841919</v>
+        <v>0.02744673962489142</v>
       </c>
       <c r="H87" t="n">
-        <v>0.5599039165206366</v>
+        <v>0.5462752274537483</v>
       </c>
     </row>
     <row r="88">
@@ -2716,25 +2716,25 @@
         <v>4336.30804020101</v>
       </c>
       <c r="B88" t="n">
-        <v>1247.814284028847</v>
+        <v>1267.988627645877</v>
       </c>
       <c r="C88" t="n">
-        <v>1.631542138855743</v>
+        <v>1.644975472364195</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0006390176016491505</v>
+        <v>0.0006490309196512755</v>
       </c>
       <c r="E88" t="n">
-        <v>1.013098431356209</v>
+        <v>1.014038813017669</v>
       </c>
       <c r="F88" t="n">
-        <v>0.5775152628413831</v>
+        <v>0.5670024365268487</v>
       </c>
       <c r="G88" t="n">
-        <v>0.02950064692552992</v>
+        <v>0.02766201508707306</v>
       </c>
       <c r="H88" t="n">
-        <v>0.5614393385757471</v>
+        <v>0.5477732756145921</v>
       </c>
     </row>
     <row r="89">
@@ -2742,25 +2742,25 @@
         <v>4386.55929648241</v>
       </c>
       <c r="B89" t="n">
-        <v>1259.936709075931</v>
+        <v>1280.503892999635</v>
       </c>
       <c r="C89" t="n">
-        <v>1.637265761857522</v>
+        <v>1.65088972644307</v>
       </c>
       <c r="D89" t="n">
-        <v>0.0006346885295052332</v>
+        <v>0.0006443452296007576</v>
       </c>
       <c r="E89" t="n">
-        <v>1.012953567562153</v>
+        <v>1.013893212445722</v>
       </c>
       <c r="F89" t="n">
-        <v>0.5735353859961385</v>
+        <v>0.5630456516142339</v>
       </c>
       <c r="G89" t="n">
-        <v>0.02973607397740457</v>
+        <v>0.02787613411205593</v>
       </c>
       <c r="H89" t="n">
-        <v>0.5629819065050538</v>
+        <v>0.5492782957110425</v>
       </c>
     </row>
     <row r="90">
@@ -2768,25 +2768,25 @@
         <v>4436.81055276382</v>
       </c>
       <c r="B90" t="n">
-        <v>1272.003638591835</v>
+        <v>1292.963766313648</v>
       </c>
       <c r="C90" t="n">
-        <v>1.642963182552624</v>
+        <v>1.65677780428135</v>
       </c>
       <c r="D90" t="n">
-        <v>0.0006304857638254461</v>
+        <v>0.0006397953431932049</v>
       </c>
       <c r="E90" t="n">
-        <v>1.012807413460661</v>
+        <v>1.013746317323047</v>
       </c>
       <c r="F90" t="n">
-        <v>0.5696390279602228</v>
+        <v>0.5591722709873673</v>
       </c>
       <c r="G90" t="n">
-        <v>0.02996998303042605</v>
+        <v>0.0280890876387804</v>
       </c>
       <c r="H90" t="n">
-        <v>0.5645316203085574</v>
+        <v>0.5507902877431002</v>
       </c>
     </row>
     <row r="91">
@@ -2794,25 +2794,25 @@
         <v>4487.06180904523</v>
       </c>
       <c r="B91" t="n">
-        <v>1284.01568582762</v>
+        <v>1305.368837176263</v>
       </c>
       <c r="C91" t="n">
-        <v>1.648634690488549</v>
+        <v>1.662639984496804</v>
       </c>
       <c r="D91" t="n">
-        <v>0.0006264039143949676</v>
+        <v>0.0006353755965898699</v>
       </c>
       <c r="E91" t="n">
-        <v>1.012659969051731</v>
+        <v>1.013598127649646</v>
       </c>
       <c r="F91" t="n">
-        <v>0.5658234543162098</v>
+        <v>0.5553795556631093</v>
       </c>
       <c r="G91" t="n">
-        <v>0.03020237514334835</v>
+        <v>0.02830086819097745</v>
       </c>
       <c r="H91" t="n">
-        <v>0.5660884799862576</v>
+        <v>0.5523092517107649</v>
       </c>
     </row>
     <row r="92">
@@ -2820,25 +2820,25 @@
         <v>4537.31306532663</v>
       </c>
       <c r="B92" t="n">
-        <v>1295.973453998943</v>
+        <v>1317.719686112008</v>
       </c>
       <c r="C92" t="n">
-        <v>1.654280570474567</v>
+        <v>1.668476541423969</v>
       </c>
       <c r="D92" t="n">
-        <v>0.0006224378766250851</v>
+        <v>0.0006310806178264579</v>
       </c>
       <c r="E92" t="n">
-        <v>1.012511234335363</v>
+        <v>1.013448643425517</v>
       </c>
       <c r="F92" t="n">
-        <v>0.5620860504960333</v>
+        <v>0.5516648869834062</v>
       </c>
       <c r="G92" t="n">
-        <v>0.03043325285957514</v>
+        <v>0.02851146977851662</v>
       </c>
       <c r="H92" t="n">
-        <v>0.5676524855381541</v>
+        <v>0.5538351876140366</v>
       </c>
     </row>
     <row r="93">
@@ -2846,25 +2846,25 @@
         <v>4587.56432160804</v>
       </c>
       <c r="B93" t="n">
-        <v>1307.877536464227</v>
+        <v>1330.016884716224</v>
       </c>
       <c r="C93" t="n">
-        <v>1.659901102665835</v>
+        <v>1.674287745177782</v>
       </c>
       <c r="D93" t="n">
-        <v>0.0006185828139821447</v>
+        <v>0.0006269053093317863</v>
       </c>
       <c r="E93" t="n">
-        <v>1.012361209311559</v>
+        <v>1.01329786465066</v>
       </c>
       <c r="F93" t="n">
-        <v>0.558424315253928</v>
+        <v>0.5480257600505578</v>
       </c>
       <c r="G93" t="n">
-        <v>0.03066262008658951</v>
+        <v>0.02872088780295697</v>
       </c>
       <c r="H93" t="n">
-        <v>0.5692236369642475</v>
+        <v>0.5553680954529154</v>
       </c>
     </row>
     <row r="94">
@@ -2872,25 +2872,25 @@
         <v>4637.81557788945</v>
       </c>
       <c r="B94" t="n">
-        <v>1319.728516902052</v>
+        <v>1342.260995791205</v>
       </c>
       <c r="C94" t="n">
-        <v>1.66549656264716</v>
+        <v>1.680073861717904</v>
       </c>
       <c r="D94" t="n">
-        <v>0.0006148341416291077</v>
+        <v>0.0006228448316260744</v>
       </c>
       <c r="E94" t="n">
-        <v>1.012209893980317</v>
+        <v>1.013145791325077</v>
       </c>
       <c r="F94" t="n">
-        <v>0.5548358545617875</v>
+        <v>0.5444597775879425</v>
       </c>
       <c r="G94" t="n">
-        <v>0.03089048198231449</v>
+        <v>0.02892911896724716</v>
       </c>
       <c r="H94" t="n">
-        <v>0.5708019342645376</v>
+        <v>0.5569079752274014</v>
       </c>
     </row>
     <row r="95">
@@ -2898,25 +2898,25 @@
         <v>4688.06683417085</v>
       </c>
       <c r="B95" t="n">
-        <v>1331.526969487488</v>
+        <v>1354.452573483378</v>
       </c>
       <c r="C95" t="n">
-        <v>1.671067221516249</v>
+        <v>1.685835152913556</v>
       </c>
       <c r="D95" t="n">
-        <v>0.0006111875111875311</v>
+        <v>0.0006188945881105951</v>
       </c>
       <c r="E95" t="n">
-        <v>1.012057288341638</v>
+        <v>1.012992423448766</v>
       </c>
       <c r="F95" t="n">
-        <v>0.551318375895403</v>
+        <v>0.5409646441944026</v>
       </c>
       <c r="G95" t="n">
-        <v>0.03111684484817345</v>
+        <v>0.02913616118953224</v>
       </c>
       <c r="H95" t="n">
-        <v>0.572387377439024</v>
+        <v>0.5584548269374942</v>
       </c>
     </row>
     <row r="96">
@@ -2924,25 +2924,25 @@
         <v>4738.31809045226</v>
       </c>
       <c r="B96" t="n">
-        <v>1343.273459067063</v>
+        <v>1366.592163421173</v>
       </c>
       <c r="C96" t="n">
-        <v>1.676613345966322</v>
+        <v>1.691571876608665</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0006076387965356421</v>
+        <v>0.0006150502108683266</v>
       </c>
       <c r="E96" t="n">
-        <v>1.011903392395522</v>
+        <v>1.012837761021728</v>
       </c>
       <c r="F96" t="n">
-        <v>0.5478696828826988</v>
+        <v>0.537538160963161</v>
       </c>
       <c r="G96" t="n">
-        <v>0.03134171602859322</v>
+        <v>0.0293420135209716</v>
       </c>
       <c r="H96" t="n">
-        <v>0.5739799664877073</v>
+        <v>0.5600086505831942</v>
       </c>
     </row>
     <row r="97">
@@ -2950,25 +2950,25 @@
         <v>4788.56934673367</v>
       </c>
       <c r="B97" t="n">
-        <v>1354.968541332123</v>
+        <v>1378.680302853108</v>
       </c>
       <c r="C97" t="n">
-        <v>1.682135198367966</v>
+        <v>1.697284286687118</v>
       </c>
       <c r="D97" t="n">
-        <v>0.0006041840805644743</v>
+        <v>0.0006113075474009851</v>
       </c>
       <c r="E97" t="n">
-        <v>1.011748206141968</v>
+        <v>1.012681804043962</v>
       </c>
       <c r="F97" t="n">
-        <v>0.5444876702875147</v>
+        <v>0.5341782204386222</v>
       </c>
       <c r="G97" t="n">
-        <v>0.0315651038167252</v>
+        <v>0.02954667606750002</v>
       </c>
       <c r="H97" t="n">
-        <v>0.5755797014105873</v>
+        <v>0.5615694461645013</v>
       </c>
     </row>
     <row r="98">
@@ -2976,25 +2976,25 @@
         <v>4838.82060301507</v>
       </c>
       <c r="B98" t="n">
-        <v>1366.612762990347</v>
+        <v>1390.717520785851</v>
       </c>
       <c r="C98" t="n">
-        <v>1.687633036850116</v>
+        <v>1.702972633138011</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0006008196428213884</v>
+        <v>0.0006076626482341816</v>
       </c>
       <c r="E98" t="n">
-        <v>1.011591729580978</v>
+        <v>1.01252455251547</v>
       </c>
       <c r="F98" t="n">
-        <v>0.5411703193046482</v>
+        <v>0.5308828018865488</v>
       </c>
       <c r="G98" t="n">
-        <v>0.03178701736608978</v>
+        <v>0.02975014991543349</v>
       </c>
       <c r="H98" t="n">
-        <v>0.5771865822076636</v>
+        <v>0.5631372136814152</v>
       </c>
     </row>
     <row r="99">
@@ -3002,25 +3002,25 @@
         <v>4889.07185929648</v>
       </c>
       <c r="B99" t="n">
-        <v>1378.206661935282</v>
+        <v>1402.704338121944</v>
       </c>
       <c r="C99" t="n">
-        <v>1.693107115380095</v>
+        <v>1.708637162120724</v>
       </c>
       <c r="D99" t="n">
-        <v>0.0005975419479750673</v>
+        <v>0.0006041117553277652</v>
       </c>
       <c r="E99" t="n">
-        <v>1.011433962712549</v>
+        <v>1.01236600643625</v>
       </c>
       <c r="F99" t="n">
-        <v>0.5379156931438555</v>
+        <v>0.5276499668551573</v>
       </c>
       <c r="G99" t="n">
-        <v>0.03200746660791031</v>
+        <v>0.02995243706081936</v>
       </c>
       <c r="H99" t="n">
-        <v>0.5788006088789368</v>
+        <v>0.5647119531339364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>